<commit_message>
Updates as of 6/18/2019
</commit_message>
<xml_diff>
--- a/Students_test/poppj-jmp448.xlsx
+++ b/Students_test/poppj-jmp448.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15540" windowWidth="16120" xWindow="9020" yWindow="460"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15540" windowWidth="16120" xWindow="3440" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PPF 2007" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PPF 2007" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName localSheetId="0" name="_xlnm.Print_Area">'PPF 2007'!$A$1:$M$114</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -995,8 +995,8 @@
   </sheetPr>
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
-      <selection activeCell="N74" sqref="N74"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
+      <selection activeCell="I79" sqref="I79:K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" outlineLevelCol="0"/>
@@ -1013,8 +1013,8 @@
     <col customWidth="1" max="11" min="11" style="33" width="9.5"/>
     <col customWidth="1" max="12" min="12" style="33" width="5.1640625"/>
     <col customWidth="1" max="13" min="13" style="33" width="9.6640625"/>
-    <col customWidth="1" max="17" min="14" style="33" width="9.1640625"/>
-    <col customWidth="1" max="16384" min="18" style="33" width="9.1640625"/>
+    <col customWidth="1" max="21" min="14" style="33" width="9.1640625"/>
+    <col customWidth="1" max="16384" min="22" style="33" width="9.1640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1790,7 +1790,6 @@
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="4" t="n"/>
-      <c r="G75" s="33" t="n"/>
       <c r="I75" s="18" t="n"/>
       <c r="K75" s="18" t="n"/>
     </row>
@@ -2068,7 +2067,7 @@
       <c r="K98" s="10" t="n"/>
       <c r="L98" s="10" t="n"/>
       <c r="M98" s="37" t="n">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:14">

</xml_diff>